<commit_message>
finalized update to the project code
hopefully
</commit_message>
<xml_diff>
--- a/Gautham_Code/State Census Purchase Combined.xlsx
+++ b/Gautham_Code/State Census Purchase Combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gautham/Documents/CS506/CS506_Project/Gautham_Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CED8E4-5F03-B648-B34A-A2AF6207FF65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1BD6D9-F1A4-8E4C-B467-7C4EE507DEE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="27440" windowHeight="25800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A2:A52"/>
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1940,12 +1940,15 @@
         <v>1.2</v>
       </c>
       <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
         <v>1.7</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>1.6</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>93.5</v>
       </c>
       <c r="P21">
@@ -2123,12 +2126,15 @@
         <v>3.1</v>
       </c>
       <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
         <v>2.4</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>5</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>75.400000000000006</v>
       </c>
       <c r="P24">
@@ -3546,12 +3552,15 @@
         <v>1.8</v>
       </c>
       <c r="L47">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="M47">
         <v>1.9</v>
       </c>
       <c r="N47">
+        <v>1.9</v>
+      </c>
+      <c r="O47">
         <v>93.1</v>
       </c>
       <c r="P47">
@@ -3729,12 +3738,15 @@
         <v>0.8</v>
       </c>
       <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
         <v>1.7</v>
       </c>
-      <c r="M50">
+      <c r="N50">
         <v>1.5</v>
       </c>
-      <c r="N50">
+      <c r="O50">
         <v>92.3</v>
       </c>
       <c r="P50">

</xml_diff>